<commit_message>
Adjusted excel-files for import tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/puutteellisiaTietojaAutotayttoaVarten.xlsx
+++ b/src/test/resources/puutteellisiaTietojaAutotayttoaVarten.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terip1/IdeaProjects/Opetushallitus/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tahon1/OPH/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E27DC32-18B3-114D-A7C2-961C7EB35C26}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34380" yWindow="2840" windowWidth="28800" windowHeight="16060"/>
+    <workbookView xWindow="38400" yWindow="2840" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="38">
   <si>
     <t>Hakkarainen</t>
   </si>
@@ -83,9 +84,6 @@
     <t>SV</t>
   </si>
   <si>
-    <t>Ehto</t>
-  </si>
-  <si>
     <t>Ehto suomi</t>
   </si>
   <si>
@@ -123,12 +121,33 @@
   </si>
   <si>
     <t>01.01.1901</t>
+  </si>
+  <si>
+    <t>muu Muu</t>
+  </si>
+  <si>
+    <t>lvm Ehdollinen: lukuvuosimaksu maksettava määräaikaan mennessä, ennen kuin voit ilmoittautua</t>
+  </si>
+  <si>
+    <t>ttk Ehdollinen: tutkintotodistuskopio hakuperusteena olleesta tutkinnosta toimitettava määräaikaan mennessä</t>
+  </si>
+  <si>
+    <t>ltt Ehdollinen: lopullinen tutkintotodistus toimitettava määräaikaan mennessä</t>
+  </si>
+  <si>
+    <t>Testi suomi</t>
+  </si>
+  <si>
+    <t>Testi ruotsi</t>
+  </si>
+  <si>
+    <t>Testi englanti</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -293,6 +312,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1372,11 +1394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1397,7 +1419,7 @@
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -1471,7 +1493,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
@@ -1487,16 +1509,16 @@
         <v>15</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="7" t="s">
@@ -1551,18 +1573,18 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>5</v>
@@ -1571,17 +1593,11 @@
         <v>15</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="P3" s="7" t="s">
         <v>6</v>
@@ -1635,37 +1651,31 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
       <c r="O4" s="6"/>
       <c r="P4" s="7" t="s">
         <v>6</v>
@@ -1719,11 +1729,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -1733,23 +1743,17 @@
         <v>4</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
       <c r="O5" s="6"/>
       <c r="P5" s="7" t="s">
         <v>6</v>
@@ -1803,36 +1807,36 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="7" t="s">

</xml_diff>